<commit_message>
Doc 09/08/2020 st 1
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
+++ b/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
@@ -88,10 +88,16 @@
     <t>Diseñar diagrama de soporte</t>
   </si>
   <si>
+    <t>Enyor</t>
+  </si>
+  <si>
     <t>Diseñar modelo Entidad relacion</t>
   </si>
   <si>
     <t>Diseñar diagrama de contexto</t>
+  </si>
+  <si>
+    <t>Dinnibel</t>
   </si>
   <si>
     <t>Definir procesos en EP y LDP</t>
@@ -101,9 +107,6 @@
   </si>
   <si>
     <t>Definir particion Funcional</t>
-  </si>
-  <si>
-    <t>Dinnibel</t>
   </si>
   <si>
     <t>Definir especificacion de control</t>
@@ -119,9 +122,6 @@
   </si>
   <si>
     <t>Definir restricciones del sistema</t>
-  </si>
-  <si>
-    <t>Enyor</t>
   </si>
   <si>
     <t>Definir criterios de rendimiento</t>
@@ -171,9 +171,9 @@
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -219,25 +219,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,9 +234,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,36 +252,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,14 +262,6 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,23 +281,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,43 +394,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,7 +442,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +478,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,49 +520,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,55 +562,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,17 +640,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,6 +673,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -693,8 +717,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,36 +737,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -763,131 +763,131 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -925,6 +925,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1251,8 +1257,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -17820,7 +17826,7 @@
       <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="8">
         <v>44050</v>
       </c>
@@ -17833,7 +17839,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="8">
@@ -17845,10 +17851,10 @@
     </row>
     <row r="14" s="2" customFormat="1" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="8">
@@ -17860,10 +17866,10 @@
     </row>
     <row r="15" s="2" customFormat="1" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="8">
@@ -17875,12 +17881,12 @@
     </row>
     <row r="16" s="2" customFormat="1" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="8">
         <v>44052</v>
       </c>
@@ -17890,12 +17896,12 @@
     </row>
     <row r="17" s="2" customFormat="1" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="8">
         <v>44052</v>
       </c>
@@ -17905,10 +17911,10 @@
     </row>
     <row r="18" s="2" customFormat="1" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="8">
@@ -17920,10 +17926,10 @@
     </row>
     <row r="19" s="2" customFormat="1" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="8">
@@ -17935,7 +17941,7 @@
     </row>
     <row r="20" s="2" customFormat="1" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>15</v>
@@ -17950,7 +17956,7 @@
     </row>
     <row r="21" s="2" customFormat="1" ht="15.75" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -17959,12 +17965,12 @@
     </row>
     <row r="22" s="2" customFormat="1" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="8">
         <v>44054</v>
       </c>
@@ -17977,9 +17983,9 @@
         <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="8">
         <v>44054</v>
       </c>
@@ -17992,9 +17998,9 @@
         <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="8">
         <v>44054</v>
       </c>
@@ -18007,9 +18013,9 @@
         <v>38</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="8">
         <v>44055</v>
       </c>
@@ -18022,9 +18028,9 @@
         <v>39</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="8">
         <v>44055</v>
       </c>
@@ -18039,7 +18045,7 @@
       <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="8">
         <v>44055</v>
       </c>
@@ -18054,7 +18060,7 @@
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="13"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="8">
         <v>44056</v>
       </c>
@@ -18069,7 +18075,7 @@
       <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="8">
         <v>44056</v>
       </c>
@@ -18093,7 +18099,7 @@
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="8">
         <v>44057</v>
       </c>
@@ -18108,7 +18114,7 @@
       <c r="B32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="8">
         <v>44057</v>
       </c>
@@ -18123,7 +18129,7 @@
       <c r="B33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="8">
         <v>44057</v>
       </c>
@@ -18138,7 +18144,7 @@
       <c r="B34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="8">
         <v>44062</v>
       </c>
@@ -18153,7 +18159,7 @@
       <c r="B35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="8">
         <v>44063</v>
       </c>

</xml_diff>

<commit_message>
12/08/2020 12:11 am st
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
+++ b/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>TAREA</t>
   </si>
@@ -31,7 +31,7 @@
     <t>FIN</t>
   </si>
   <si>
-    <t>PLANIFICACION DEL PROYECTO</t>
+    <t>PLANIFICACION Y ANALISIS DEL PROYECTO</t>
   </si>
   <si>
     <t>Pendiente</t>
@@ -76,6 +76,9 @@
     <t>ANALISIS</t>
   </si>
   <si>
+    <t>Definir Requerimientos</t>
+  </si>
+  <si>
     <t>Definir descripcion del sistema  y objetivos</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
   </si>
   <si>
     <t>Diseñar diagrama de soporte</t>
-  </si>
-  <si>
-    <t>Enyor</t>
   </si>
   <si>
     <t>Diseñar modelo Entidad relacion</t>
@@ -133,6 +133,9 @@
     <t>Diseño arquitectonico de los procesos estrategicos</t>
   </si>
   <si>
+    <t>Enyor</t>
+  </si>
+  <si>
     <t>Definir normas de diseño</t>
   </si>
   <si>
@@ -142,7 +145,7 @@
     <t>Enlistar y definir modelo de tablas</t>
   </si>
   <si>
-    <t>Verificar todo el Modelo</t>
+    <t>Verificar todo el Diseño</t>
   </si>
   <si>
     <t>DESARROLLO Y PRUEBA</t>
@@ -160,6 +163,9 @@
     <t>Comprobar funcionamiento de los modulos</t>
   </si>
   <si>
+    <t xml:space="preserve">ENTREGA </t>
+  </si>
+  <si>
     <t>Presentar Proyecto final</t>
   </si>
 </sst>
@@ -170,10 +176,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -206,15 +212,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,6 +223,58 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,36 +301,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -305,13 +325,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -319,15 +332,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,15 +341,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,7 +400,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,7 +544,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,163 +574,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,10 +648,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -655,7 +659,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -675,17 +694,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,24 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -737,18 +732,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -760,130 +766,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1255,15 +1261,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD35"/>
+  <dimension ref="A1:XFD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="$A10:$XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.5714285714286" style="2" customWidth="1"/>
+    <col min="1" max="1" width="54.6380952380952" style="2" customWidth="1"/>
     <col min="2" max="2" width="37.5714285714286" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.4285714285714" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.5714285714286" style="2" customWidth="1"/>
@@ -17809,9 +17815,9 @@
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="8">
         <v>44050</v>
       </c>
@@ -17821,12 +17827,12 @@
     </row>
     <row r="12" s="2" customFormat="1" spans="1:5">
       <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="8">
         <v>44050</v>
       </c>
@@ -17839,22 +17845,22 @@
         <v>23</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="8">
-        <v>44051</v>
+        <v>44050</v>
       </c>
       <c r="E13" s="8">
-        <v>44051</v>
+        <v>44050</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="8">
@@ -17866,27 +17872,27 @@
     </row>
     <row r="15" s="2" customFormat="1" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="8">
-        <v>44052</v>
+        <v>44051</v>
       </c>
       <c r="E15" s="8">
-        <v>44052</v>
+        <v>44051</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="8">
         <v>44052</v>
       </c>
@@ -17896,7 +17902,7 @@
     </row>
     <row r="17" s="2" customFormat="1" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>15</v>
@@ -17911,25 +17917,25 @@
     </row>
     <row r="18" s="2" customFormat="1" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="8">
-        <v>44053</v>
+        <v>44052</v>
       </c>
       <c r="E18" s="8">
-        <v>44053</v>
+        <v>44052</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="8">
@@ -17941,10 +17947,10 @@
     </row>
     <row r="20" s="2" customFormat="1" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="8">
@@ -17954,33 +17960,33 @@
         <v>44053</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A21" s="4" t="s">
+    <row r="21" s="2" customFormat="1" spans="1:5">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="8">
+        <v>44053</v>
+      </c>
+      <c r="E21" s="8">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" s="2" customFormat="1" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="8">
-        <v>44054</v>
-      </c>
-      <c r="E22" s="8">
-        <v>44054</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" s="2" customFormat="1" spans="1:5">
       <c r="A23" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>8</v>
@@ -17995,12 +18001,12 @@
     </row>
     <row r="24" s="2" customFormat="1" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="8">
         <v>44054</v>
       </c>
@@ -18010,25 +18016,25 @@
     </row>
     <row r="25" s="2" customFormat="1" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="8">
-        <v>44055</v>
+        <v>44054</v>
       </c>
       <c r="E25" s="8">
-        <v>44055</v>
+        <v>44054</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="8">
@@ -18043,14 +18049,14 @@
         <v>40</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="8">
         <v>44055</v>
       </c>
       <c r="E27" s="8">
-        <v>44056</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" spans="1:5">
@@ -18058,11 +18064,11 @@
         <v>41</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="8">
-        <v>44056</v>
+        <v>44055</v>
       </c>
       <c r="E28" s="8">
         <v>44056</v>
@@ -18073,7 +18079,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="8">
@@ -18083,31 +18089,31 @@
         <v>44056</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="1:5">
-      <c r="A30" s="4" t="s">
+    <row r="30" s="2" customFormat="1" spans="1:5">
+      <c r="A30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="B30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="8">
+        <v>44056</v>
+      </c>
+      <c r="E30" s="8">
+        <v>44056</v>
+      </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="6" t="s">
+    <row r="31" s="2" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="8">
-        <v>44057</v>
-      </c>
-      <c r="E31" s="8">
-        <v>44062</v>
-      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" s="2" customFormat="1" spans="1:5">
       <c r="A32" s="6" t="s">
         <v>45</v>
       </c>
@@ -18122,7 +18128,7 @@
         <v>44062</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" s="2" customFormat="1" spans="1:5">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -18137,7 +18143,7 @@
         <v>44062</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" s="2" customFormat="1" spans="1:5">
       <c r="A34" s="6" t="s">
         <v>47</v>
       </c>
@@ -18146,13 +18152,13 @@
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="8">
-        <v>44062</v>
+        <v>44057</v>
       </c>
       <c r="E34" s="8">
         <v>44062</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" s="2" customFormat="1" spans="1:5">
       <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
@@ -18161,18 +18167,43 @@
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="8">
+        <v>44062</v>
+      </c>
+      <c r="E35" s="8">
+        <v>44062</v>
+      </c>
+    </row>
+    <row r="36" s="2" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="8">
         <v>44063</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E37" s="8">
         <v>44063</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A36:E36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update 2.- DIAGRAMA DE GANTT.xlsx
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
+++ b/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enyor Peralta\Documents\GitHub\ElFinal\DOCUMENTACION\I. PLANIFICACION DEL PROYECTO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BE1655-6700-4D95-8E49-846AD268BC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,16 +178,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,152 +212,8 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,7 +240,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.05"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,194 +256,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -645,251 +317,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -906,9 +336,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -918,7 +345,7 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1">
@@ -936,68 +363,27 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1255,31 +641,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="$A10:$XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.6380952380952" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.5714285714286" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.4285714285714" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5714285714286" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5714285714286" style="2" customWidth="1"/>
-    <col min="6" max="7" width="9.14285714285714" style="2"/>
-    <col min="8" max="8" width="11.2857142857143" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.14285714285714" style="2"/>
+    <col min="1" max="1" width="54.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="11.28515625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.75" spans="1:16384">
+    <row r="1" spans="1:16384" s="1" customFormat="1" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -17675,525 +17061,525 @@
       <c r="XFC1" s="2"/>
       <c r="XFD1" s="2"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="15.75" spans="1:8">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:16384" ht="15.75">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:8">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:16384">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7">
         <v>44050</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>44050</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:8">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:16384">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8">
+      <c r="C4" s="9"/>
+      <c r="D4" s="7">
         <v>44050</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>44050</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:5">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:16384">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8">
+      <c r="C5" s="9"/>
+      <c r="D5" s="7">
         <v>44050</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:5">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:16384">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8">
+      <c r="C6" s="9"/>
+      <c r="D6" s="7">
         <v>44050</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="1" spans="1:5">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:16384">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8">
+      <c r="C7" s="9"/>
+      <c r="D7" s="7">
         <v>44050</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" spans="1:5">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:16384">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8">
+      <c r="C8" s="9"/>
+      <c r="D8" s="7">
         <v>44050</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" spans="1:5">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:16384">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8">
+      <c r="C9" s="9"/>
+      <c r="D9" s="7">
         <v>44050</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:16384" ht="15.75">
+      <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
-    <row r="11" s="2" customFormat="1" spans="1:5">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:16384">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8">
+      <c r="C11" s="9"/>
+      <c r="D11" s="7">
         <v>44050</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" spans="1:5">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:16384">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="8">
+      <c r="C12" s="11"/>
+      <c r="D12" s="7">
         <v>44050</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" spans="1:5">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:16384">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="8">
+      <c r="C13" s="12"/>
+      <c r="D13" s="7">
         <v>44050</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>44050</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" spans="1:5">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:16384">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="8">
+      <c r="C14" s="11"/>
+      <c r="D14" s="7">
         <v>44051</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>44051</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" spans="1:5">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:16384">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="8">
+      <c r="C15" s="11"/>
+      <c r="D15" s="7">
         <v>44051</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>44051</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" spans="1:5">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:16384">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="8">
+      <c r="C16" s="11"/>
+      <c r="D16" s="7">
         <v>44052</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>44052</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" spans="1:5">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="8">
+      <c r="C17" s="12"/>
+      <c r="D17" s="7">
         <v>44052</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>44052</v>
       </c>
     </row>
-    <row r="18" s="2" customFormat="1" spans="1:5">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="8">
+      <c r="C18" s="12"/>
+      <c r="D18" s="7">
         <v>44052</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>44052</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" spans="1:5">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="8">
+      <c r="C19" s="11"/>
+      <c r="D19" s="7">
         <v>44053</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>44053</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" spans="1:5">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="8">
+      <c r="C20" s="11"/>
+      <c r="D20" s="7">
         <v>44053</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>44053</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" spans="1:5">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="8">
+      <c r="C21" s="11"/>
+      <c r="D21" s="7">
         <v>44053</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>44053</v>
       </c>
     </row>
-    <row r="22" s="2" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:5" ht="15.75">
+      <c r="A22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
-    <row r="23" s="2" customFormat="1" spans="1:5">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="8">
+      <c r="C23" s="13"/>
+      <c r="D23" s="7">
         <v>44054</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>44054</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" spans="1:5">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="8">
+      <c r="C24" s="13"/>
+      <c r="D24" s="7">
         <v>44054</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>44054</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" spans="1:5">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="8">
+      <c r="C25" s="14"/>
+      <c r="D25" s="7">
         <v>44054</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>44054</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="1" spans="1:5">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="8">
+      <c r="C26" s="14"/>
+      <c r="D26" s="7">
         <v>44055</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>44055</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" spans="1:5">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="8">
+      <c r="C27" s="14"/>
+      <c r="D27" s="7">
         <v>44055</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>44055</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:5">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="8">
+      <c r="C28" s="14"/>
+      <c r="D28" s="7">
         <v>44055</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <v>44056</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:5">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="8">
+      <c r="C29" s="14"/>
+      <c r="D29" s="7">
         <v>44056</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>44056</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" spans="1:5">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="8">
+      <c r="C30" s="14"/>
+      <c r="D30" s="7">
         <v>44056</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>44056</v>
       </c>
     </row>
-    <row r="31" s="2" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:5" ht="15.75">
+      <c r="A31" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
-    <row r="32" s="2" customFormat="1" spans="1:5">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="8">
+      <c r="C32" s="14"/>
+      <c r="D32" s="7">
         <v>44057</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>44062</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="1" spans="1:5">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="8">
+      <c r="C33" s="14"/>
+      <c r="D33" s="7">
         <v>44057</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>44062</v>
       </c>
     </row>
-    <row r="34" s="2" customFormat="1" spans="1:5">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="8">
+      <c r="C34" s="14"/>
+      <c r="D34" s="7">
         <v>44057</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>44062</v>
       </c>
     </row>
-    <row r="35" s="2" customFormat="1" spans="1:5">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="8">
+      <c r="C35" s="14"/>
+      <c r="D35" s="7">
         <v>44062</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>44062</v>
       </c>
     </row>
-    <row r="36" s="2" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:5" ht="15.75">
+      <c r="A36" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="8">
+      <c r="C37" s="14"/>
+      <c r="D37" s="7">
         <v>44063</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>44063</v>
       </c>
     </row>
@@ -18206,6 +17592,5 @@
     <mergeCell ref="A36:E36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ep - Cambios en el Diagrama de Gant
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
+++ b/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enyor Peralta\Documents\GitHub\ElFinal\DOCUMENTACION\I. PLANIFICACION DEL PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BE1655-6700-4D95-8E49-846AD268BC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F4C375-6187-4E74-86C1-CF6842B1A64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -650,7 +650,7 @@
   <dimension ref="A1:XFD37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17248,7 +17248,7 @@
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="7">
         <v>44051</v>
       </c>
@@ -17263,7 +17263,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="7">
         <v>44051</v>
       </c>
@@ -17278,7 +17278,7 @@
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="7">
         <v>44052</v>
       </c>
@@ -17338,7 +17338,7 @@
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="7">
         <v>44053</v>
       </c>
@@ -17422,7 +17422,7 @@
       <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="7">
         <v>44055</v>
       </c>

</xml_diff>

<commit_message>
Documentacion st 17/08/2020 15:45pm
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
+++ b/DOCUMENTACION/I. PLANIFICACION DEL PROYECTO/2.- DIAGRAMA DE GANTT.xlsx
@@ -1,34 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enyor Peralta\Documents\GitHub\ElFinal\DOCUMENTACION\I. PLANIFICACION DEL PROYECTO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F4C375-6187-4E74-86C1-CF6842B1A64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>TAREA</t>
   </si>
   <si>
     <t>ASIGNADA A</t>
-  </si>
-  <si>
-    <t>PROGRESO</t>
   </si>
   <si>
     <t>INICIO</t>
@@ -40,7 +31,16 @@
     <t>PLANIFICACION Y ANALISIS DEL PROYECTO</t>
   </si>
   <si>
-    <t>Pendiente</t>
+    <t>Definir Requerimientos</t>
+  </si>
+  <si>
+    <t>Cliente y Equipo de Trabajo</t>
+  </si>
+  <si>
+    <t>Definir Metodo de Integracion</t>
+  </si>
+  <si>
+    <t>20-Agu-2020</t>
   </si>
   <si>
     <t>Definir ambito del software</t>
@@ -49,13 +49,10 @@
     <t>Sugeiri</t>
   </si>
   <si>
-    <t>En Proceso</t>
+    <t>21-Agu-2020</t>
   </si>
   <si>
     <t>Definir las ventajas</t>
-  </si>
-  <si>
-    <t>Terminado</t>
   </si>
   <si>
     <t>Seleccionar Modelo y Tipo de Equipo</t>
@@ -64,10 +61,16 @@
     <t>Equipo Trabajo</t>
   </si>
   <si>
+    <t>22-Agu-2020</t>
+  </si>
+  <si>
     <t>Identificar las tareas a realizar</t>
   </si>
   <si>
     <t>Equipo de Trabajo</t>
+  </si>
+  <si>
+    <t>23-Agu-2020</t>
   </si>
   <si>
     <t>Distribuir responsabilidades</t>
@@ -76,19 +79,28 @@
     <t>Elaborar presupuesto</t>
   </si>
   <si>
-    <t>Analizar diagrama de Gantt</t>
+    <t>25-Agu-2020</t>
+  </si>
+  <si>
+    <t>27-Agu-2020</t>
+  </si>
+  <si>
+    <t>Reunion para analisis y evaluacion de avances</t>
+  </si>
+  <si>
+    <t>28-Agu-2020</t>
   </si>
   <si>
     <t>ANALISIS</t>
   </si>
   <si>
-    <t>Definir Requerimientos</t>
+    <t>30-Agu-2020</t>
   </si>
   <si>
     <t>Definir descripcion del sistema  y objetivos</t>
   </si>
   <si>
-    <t>Luisa</t>
+    <t>31-Agu-2020</t>
   </si>
   <si>
     <t>Definir elementos estrategicos</t>
@@ -124,6 +136,12 @@
     <t>Verificar todo el analisis</t>
   </si>
   <si>
+    <t>Evaluacion de Avances</t>
+  </si>
+  <si>
+    <t>Adaptacion de Cambios Solicitados</t>
+  </si>
+  <si>
     <t>DISEÑO</t>
   </si>
   <si>
@@ -134,6 +152,9 @@
   </si>
   <si>
     <t>Enlistar modulos y programas</t>
+  </si>
+  <si>
+    <t>Luisa</t>
   </si>
   <si>
     <t>Diseño arquitectonico de los procesos estrategicos</t>
@@ -157,10 +178,22 @@
     <t>DESARROLLO Y PRUEBA</t>
   </si>
   <si>
-    <t>Cargar datos de configuraciones a la base de datos</t>
+    <t>Crear Base de datos</t>
   </si>
   <si>
-    <t>Programar el sitio web en Pycharm con Html y Python</t>
+    <t>Programar Mantenimiento de Articulo y sus derivados</t>
+  </si>
+  <si>
+    <t>Programar Mantenimiento de Recetas y sus derivados</t>
+  </si>
+  <si>
+    <t>Almacenar Equivalencia de Unidades de Medida</t>
+  </si>
+  <si>
+    <t>Programar Configuracion de Formula de recetas</t>
+  </si>
+  <si>
+    <t>Diseñar funciones necesarias para formula de receta</t>
   </si>
   <si>
     <t>Desarrollar algoritmos de las partes inteligentes</t>
@@ -169,21 +202,30 @@
     <t>Comprobar funcionamiento de los modulos</t>
   </si>
   <si>
-    <t xml:space="preserve">ENTREGA </t>
+    <t>Diseñar manuales de instalacion</t>
   </si>
   <si>
-    <t>Presentar Proyecto final</t>
+    <t>Diseñar manuales de configuracion</t>
+  </si>
+  <si>
+    <t>Diseñar manuales de Uso</t>
+  </si>
+  <si>
+    <t>Entrega de Avances</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,28 +234,171 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF002060"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,30 +419,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.05"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -281,109 +634,331 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -641,31 +1216,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:XFA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="11.28515625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="54.6380952380952" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.5714285714286" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.5714285714286" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5714285714286" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" ht="15.75">
+    <row r="1" s="1" customFormat="1" ht="20.25" spans="1:16381">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -678,9 +1250,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -17057,540 +17627,678 @@
       <c r="XEY1" s="2"/>
       <c r="XEZ1" s="2"/>
       <c r="XFA1" s="2"/>
-      <c r="XFB1" s="2"/>
-      <c r="XFC1" s="2"/>
-      <c r="XFD1" s="2"/>
     </row>
-    <row r="2" spans="1:16384" ht="15.75">
-      <c r="A2" s="15" t="s">
+    <row r="2" s="2" customFormat="1" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="6">
+        <v>44050</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44058</v>
+      </c>
     </row>
-    <row r="3" spans="1:16384">
-      <c r="A3" s="5" t="s">
+    <row r="4" s="2" customFormat="1" spans="1:4">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>44059</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E3" s="7">
-        <v>44050</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:4">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:16384">
-      <c r="A4" s="5" t="s">
+    <row r="6" s="2" customFormat="1" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E4" s="7">
-        <v>44050</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:16384">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="7" s="2" customFormat="1" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E5" s="7">
-        <v>44050</v>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16384">
-      <c r="A6" s="5" t="s">
+    <row r="8" s="2" customFormat="1" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6">
+        <v>44067</v>
+      </c>
+      <c r="D9" s="6">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" spans="1:4">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <v>44075</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44081</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6">
+        <v>44082</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6">
+        <v>44090</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44099</v>
+      </c>
+    </row>
+    <row r="18" s="2" customFormat="1" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>44100</v>
+      </c>
+      <c r="D18" s="6">
+        <v>44106</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6">
+        <v>44107</v>
+      </c>
+      <c r="D19" s="6">
+        <v>44124</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="1" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6">
+        <v>44125</v>
+      </c>
+      <c r="D20" s="6">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6">
+        <v>44139</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6">
+        <v>44151</v>
+      </c>
+      <c r="D22" s="6">
+        <v>44156</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="1" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="6">
+        <v>44157</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44157</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6">
+        <v>44158</v>
+      </c>
+      <c r="D24" s="6">
+        <v>44158</v>
+      </c>
+    </row>
+    <row r="25" s="2" customFormat="1" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="6">
+        <v>44159</v>
+      </c>
+      <c r="D25" s="6">
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="26" s="2" customFormat="1" spans="1:4">
+      <c r="A26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" s="2" customFormat="1" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6">
+        <v>44163</v>
+      </c>
+      <c r="D27" s="6">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="28" s="2" customFormat="1" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="6">
+        <v>44166</v>
+      </c>
+      <c r="D28" s="6">
+        <v>44170</v>
+      </c>
+    </row>
+    <row r="29" s="2" customFormat="1" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44171</v>
+      </c>
+      <c r="D29" s="6">
+        <v>44180</v>
+      </c>
+    </row>
+    <row r="30" s="2" customFormat="1" ht="37.5" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="6">
+        <v>44181</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44185</v>
+      </c>
+    </row>
+    <row r="31" s="2" customFormat="1" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="6">
+        <v>44186</v>
+      </c>
+      <c r="D31" s="6">
+        <v>44192</v>
+      </c>
+    </row>
+    <row r="32" s="2" customFormat="1" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E6" s="7">
-        <v>44050</v>
+      <c r="C32" s="6">
+        <v>44206</v>
+      </c>
+      <c r="D32" s="6">
+        <v>44224</v>
       </c>
     </row>
-    <row r="7" spans="1:16384">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E7" s="7">
-        <v>44050</v>
+    <row r="33" s="2" customFormat="1" spans="1:4">
+      <c r="A33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="6">
+        <v>44225</v>
+      </c>
+      <c r="D33" s="6">
+        <v>44237</v>
       </c>
     </row>
-    <row r="8" spans="1:16384">
-      <c r="A8" s="5" t="s">
+    <row r="34" s="2" customFormat="1" spans="1:4">
+      <c r="A34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="6">
+        <v>44238</v>
+      </c>
+      <c r="D34" s="6">
+        <v>44238</v>
+      </c>
+    </row>
+    <row r="35" s="2" customFormat="1" spans="1:4">
+      <c r="A35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="6">
+        <v>44239</v>
+      </c>
+      <c r="D35" s="6">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="36" s="2" customFormat="1" spans="1:4">
+      <c r="A36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E8" s="7">
-        <v>44050</v>
+      <c r="C36" s="6">
+        <v>44240</v>
+      </c>
+      <c r="D36" s="6">
+        <v>44244</v>
       </c>
     </row>
-    <row r="9" spans="1:16384">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E9" s="7">
-        <v>44050</v>
-      </c>
+    <row r="37" s="2" customFormat="1" spans="1:4">
+      <c r="A37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
     </row>
-    <row r="10" spans="1:16384" ht="15.75">
-      <c r="A10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+    <row r="38" s="2" customFormat="1" spans="1:4">
+      <c r="A38" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="6">
+        <v>44246</v>
+      </c>
+      <c r="D38" s="6">
+        <v>44246</v>
+      </c>
     </row>
-    <row r="11" spans="1:16384">
-      <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E11" s="7">
-        <v>44050</v>
+    <row r="39" s="2" customFormat="1" ht="37.5" spans="1:4">
+      <c r="A39" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6">
+        <v>44247</v>
+      </c>
+      <c r="D39" s="6">
+        <v>44252</v>
       </c>
     </row>
-    <row r="12" spans="1:16384">
-      <c r="A12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E12" s="7">
-        <v>44050</v>
+    <row r="40" s="2" customFormat="1" ht="37.5" spans="1:4">
+      <c r="A40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="6">
+        <v>44253</v>
+      </c>
+      <c r="D40" s="6">
+        <v>44255</v>
       </c>
     </row>
-    <row r="13" spans="1:16384">
-      <c r="A13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="7">
-        <v>44050</v>
-      </c>
-      <c r="E13" s="7">
-        <v>44050</v>
+    <row r="41" s="2" customFormat="1" spans="1:4">
+      <c r="A41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6">
+        <v>44256</v>
+      </c>
+      <c r="D41" s="6">
+        <v>44256</v>
       </c>
     </row>
-    <row r="14" spans="1:16384">
-      <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="7">
-        <v>44051</v>
-      </c>
-      <c r="E14" s="7">
-        <v>44051</v>
+    <row r="42" s="2" customFormat="1" spans="1:4">
+      <c r="A42" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="6">
+        <v>44257</v>
+      </c>
+      <c r="D42" s="6">
+        <v>44262</v>
       </c>
     </row>
-    <row r="15" spans="1:16384">
-      <c r="A15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="7">
-        <v>44051</v>
-      </c>
-      <c r="E15" s="7">
-        <v>44051</v>
+    <row r="43" s="2" customFormat="1" ht="37.5" spans="1:4">
+      <c r="A43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="6">
+        <v>44263</v>
+      </c>
+      <c r="D43" s="6">
+        <v>44270</v>
       </c>
     </row>
-    <row r="16" spans="1:16384">
-      <c r="A16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="7">
-        <v>44052</v>
-      </c>
-      <c r="E16" s="7">
-        <v>44052</v>
+    <row r="44" s="2" customFormat="1" spans="1:4">
+      <c r="A44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="6">
+        <v>44271</v>
+      </c>
+      <c r="D44" s="6">
+        <v>44296</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="7">
-        <v>44052</v>
-      </c>
-      <c r="E17" s="7">
-        <v>44052</v>
+    <row r="45" s="2" customFormat="1" spans="1:4">
+      <c r="A45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="6">
+        <v>44297</v>
+      </c>
+      <c r="D45" s="6">
+        <v>44304</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="7">
-        <v>44052</v>
-      </c>
-      <c r="E18" s="7">
-        <v>44052</v>
+    <row r="46" s="2" customFormat="1" spans="1:4">
+      <c r="A46" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="6">
+        <v>44306</v>
+      </c>
+      <c r="D46" s="6">
+        <v>44308</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="7">
-        <v>44053</v>
-      </c>
-      <c r="E19" s="7">
-        <v>44053</v>
+    <row r="47" s="2" customFormat="1" spans="1:4">
+      <c r="A47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="6">
+        <v>44309</v>
+      </c>
+      <c r="D47" s="6">
+        <v>44311</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="7">
-        <v>44053</v>
-      </c>
-      <c r="E20" s="7">
-        <v>44053</v>
+    <row r="48" s="2" customFormat="1" spans="1:4">
+      <c r="A48" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="6">
+        <v>44312</v>
+      </c>
+      <c r="D48" s="6">
+        <v>44317</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="7">
-        <v>44053</v>
-      </c>
-      <c r="E21" s="7">
-        <v>44053</v>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="6">
+        <v>44319</v>
+      </c>
+      <c r="D49" s="6">
+        <v>44319</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75">
-      <c r="A22" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="7">
-        <v>44054</v>
-      </c>
-      <c r="E23" s="7">
-        <v>44054</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="7">
-        <v>44054</v>
-      </c>
-      <c r="E24" s="7">
-        <v>44054</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="7">
-        <v>44054</v>
-      </c>
-      <c r="E25" s="7">
-        <v>44054</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="7">
-        <v>44055</v>
-      </c>
-      <c r="E26" s="7">
-        <v>44055</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="7">
-        <v>44055</v>
-      </c>
-      <c r="E27" s="7">
-        <v>44055</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="7">
-        <v>44055</v>
-      </c>
-      <c r="E28" s="7">
-        <v>44056</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="7">
-        <v>44056</v>
-      </c>
-      <c r="E29" s="7">
-        <v>44056</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="7">
-        <v>44056</v>
-      </c>
-      <c r="E30" s="7">
-        <v>44056</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75">
-      <c r="A31" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="7">
-        <v>44057</v>
-      </c>
-      <c r="E32" s="7">
-        <v>44062</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="7">
-        <v>44057</v>
-      </c>
-      <c r="E33" s="7">
-        <v>44062</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="7">
-        <v>44057</v>
-      </c>
-      <c r="E34" s="7">
-        <v>44062</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="7">
-        <v>44062</v>
-      </c>
-      <c r="E35" s="7">
-        <v>44062</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75">
-      <c r="A36" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="7">
-        <v>44063</v>
-      </c>
-      <c r="E37" s="7">
-        <v>44063</v>
+      <c r="B50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="6">
+        <v>44320</v>
+      </c>
+      <c r="D50" s="6">
+        <v>44336</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A36:E36"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>